<commit_message>
Corrected pH inputs after talk with Irith
</commit_message>
<xml_diff>
--- a/2022_more_separation/inputs/inputs.xlsx
+++ b/2022_more_separation/inputs/inputs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\au583430\OneDrive - Aarhus Universitet\Dokumenter\GitHub\AU-myndighedsbetjening\2022_more_separation\inputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2" documentId="11_C7D6A3A17A5F2DAE79EA988F53CAEA9664EF159B" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{9AF3A76D-E25E-4ADE-BFF9-8FFE023CF172}"/>
+  <xr:revisionPtr revIDLastSave="10" documentId="11_C7D6A3A17A5F2DAE79EA988F53CAEA9664EF159B" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{7FD89513-544E-4E34-96AA-104734B4C135}"/>
   <bookViews>
-    <workbookView xWindow="-38520" yWindow="-3255" windowWidth="38640" windowHeight="21240" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2595" yWindow="135" windowWidth="28800" windowHeight="15435" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Slurry source" sheetId="1" r:id="rId1"/>
@@ -596,7 +596,7 @@
   <dimension ref="A1:A8"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="N4" sqref="N4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.140625" defaultRowHeight="12.75"/>
@@ -608,37 +608,37 @@
     </row>
     <row r="2" spans="1:1">
       <c r="A2">
-        <v>8.1999999999999993</v>
+        <v>8.3000000000000007</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3">
-        <v>7.95</v>
+        <v>8.1</v>
       </c>
     </row>
     <row r="4" spans="1:1">
       <c r="A4">
-        <v>7.8</v>
+        <v>7.9</v>
       </c>
     </row>
     <row r="5" spans="1:1">
       <c r="A5">
-        <v>7.6</v>
+        <v>7.7</v>
       </c>
     </row>
     <row r="6" spans="1:1">
       <c r="A6">
-        <v>7.4</v>
+        <v>7.5</v>
       </c>
     </row>
     <row r="7" spans="1:1">
       <c r="A7">
-        <v>7.2</v>
+        <v>7.3</v>
       </c>
     </row>
     <row r="8" spans="1:1">
       <c r="A8">
-        <v>7</v>
+        <v>7.1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Changed . to , in plot, added scale package
</commit_message>
<xml_diff>
--- a/2022_more_separation/inputs/inputs.xlsx
+++ b/2022_more_separation/inputs/inputs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\au583430\OneDrive - Aarhus Universitet\Dokumenter\GitHub\AU-myndighedsbetjening\2022_more_separation\inputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="10" documentId="11_C7D6A3A17A5F2DAE79EA988F53CAEA9664EF159B" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{7FD89513-544E-4E34-96AA-104734B4C135}"/>
+  <xr:revisionPtr revIDLastSave="11" documentId="11_C7D6A3A17A5F2DAE79EA988F53CAEA9664EF159B" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{80EFBB55-FC85-47E3-B3C3-747F30BB03BE}"/>
   <bookViews>
-    <workbookView xWindow="2595" yWindow="135" windowWidth="28800" windowHeight="15435" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-37275" yWindow="-2010" windowWidth="28800" windowHeight="15435" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Slurry source" sheetId="1" r:id="rId1"/>
@@ -593,10 +593,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:A8"/>
+  <dimension ref="A1:A9"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="N4" sqref="N4"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.140625" defaultRowHeight="12.75"/>
@@ -639,6 +639,11 @@
     <row r="8" spans="1:1">
       <c r="A8">
         <v>7.1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1">
+      <c r="A9">
+        <v>6.9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>